<commit_message>
Now correctly codes Slowbro
</commit_message>
<xml_diff>
--- a/research-log/pokelog.xlsx
+++ b/research-log/pokelog.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24660" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="24960" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="650">
   <si>
     <t>Sandshrew</t>
   </si>
@@ -1182,15 +1182,6 @@
     <t>Luxio</t>
   </si>
   <si>
-    <t xml:space="preserve">Pokémon </t>
-  </si>
-  <si>
-    <t>Mega Pokémon</t>
-  </si>
-  <si>
-    <t>NFE</t>
-  </si>
-  <si>
     <t>Abomasnow</t>
   </si>
   <si>
@@ -1518,9 +1509,6 @@
     <t>Gothitelle</t>
   </si>
   <si>
-    <t>Gourgeist (all forms)</t>
-  </si>
-  <si>
     <t>Hawlucha</t>
   </si>
   <si>
@@ -1620,9 +1608,6 @@
     <t>Meloetta</t>
   </si>
   <si>
-    <t>Meowstic (Both Male and Female)</t>
-  </si>
-  <si>
     <t>Mienshao</t>
   </si>
   <si>
@@ -1695,21 +1680,6 @@
     <t>Reuniclus</t>
   </si>
   <si>
-    <t>Rotom (Normal form)</t>
-  </si>
-  <si>
-    <t>Rotom-C (Lawn Mower form)</t>
-  </si>
-  <si>
-    <t>Rotom-F (Freezer form)</t>
-  </si>
-  <si>
-    <t>Rotom-H (Heat Form)</t>
-  </si>
-  <si>
-    <t>Rotom-S (Fan form)</t>
-  </si>
-  <si>
     <t>Rotom-W</t>
   </si>
   <si>
@@ -1839,18 +1809,12 @@
     <t>Wobbuffet</t>
   </si>
   <si>
-    <t>Wormadam (All Forms)</t>
-  </si>
-  <si>
     <t>Xatu</t>
   </si>
   <si>
     <t>Zebstrika</t>
   </si>
   <si>
-    <t>MegaPokémon</t>
-  </si>
-  <si>
     <t xml:space="preserve">Charizard </t>
   </si>
   <si>
@@ -1972,6 +1936,39 @@
   </si>
   <si>
     <t>Venusaurite</t>
+  </si>
+  <si>
+    <t>Gourgeist </t>
+  </si>
+  <si>
+    <t>Meowstic</t>
+  </si>
+  <si>
+    <t>Rotom </t>
+  </si>
+  <si>
+    <t>Rotom-C </t>
+  </si>
+  <si>
+    <t>Rotom-F</t>
+  </si>
+  <si>
+    <t>Rotom-H</t>
+  </si>
+  <si>
+    <t>Rotom-S </t>
+  </si>
+  <si>
+    <t>poke</t>
+  </si>
+  <si>
+    <t>mpoke</t>
+  </si>
+  <si>
+    <t>nfe</t>
+  </si>
+  <si>
+    <t>megapokform</t>
   </si>
 </sst>
 </file>
@@ -2311,7 +2308,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2319,10 +2316,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N414"/>
+  <dimension ref="A1:N416"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2335,16 +2332,16 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>387</v>
+        <v>646</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>388</v>
+        <v>647</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>389</v>
+        <v>648</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>609</v>
+        <v>649</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>141</v>
@@ -2374,21 +2371,21 @@
         <v>385</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>611</v>
+        <v>599</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>25</v>
@@ -2418,21 +2415,21 @@
         <v>25</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>52</v>
@@ -2462,7 +2459,7 @@
         <v>365</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>613</v>
+        <v>601</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2470,10 +2467,10 @@
         <v>163</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>25</v>
@@ -2506,7 +2503,7 @@
         <v>200</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>614</v>
+        <v>602</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2514,10 +2511,10 @@
         <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>52</v>
@@ -2550,7 +2547,7 @@
         <v>363</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>615</v>
+        <v>603</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2558,13 +2555,13 @@
         <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>241</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>121</v>
@@ -2594,18 +2591,18 @@
         <v>83</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>616</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>319</v>
@@ -2638,21 +2635,21 @@
         <v>210</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>617</v>
+        <v>605</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="3" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>63</v>
@@ -2682,7 +2679,7 @@
         <v>178</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>618</v>
+        <v>606</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -2690,13 +2687,13 @@
         <v>319</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>123</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>50</v>
@@ -2723,21 +2720,21 @@
         <v>366</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>619</v>
+        <v>607</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>139</v>
@@ -2764,15 +2761,15 @@
         <v>376</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>620</v>
+        <v>608</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>260</v>
@@ -2805,15 +2802,15 @@
         <v>206</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>621</v>
+        <v>609</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>94</v>
@@ -2846,7 +2843,7 @@
         <v>381</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>622</v>
+        <v>610</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -2854,7 +2851,7 @@
         <v>237</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>30</v>
@@ -2887,7 +2884,7 @@
         <v>369</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>623</v>
+        <v>611</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -2895,13 +2892,13 @@
         <v>281</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>206</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>610</v>
+        <v>598</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>86</v>
@@ -2928,7 +2925,7 @@
         <v>97</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>624</v>
+        <v>612</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -2936,10 +2933,10 @@
         <v>122</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>11</v>
@@ -2969,7 +2966,7 @@
         <v>303</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>625</v>
+        <v>613</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -2977,13 +2974,13 @@
         <v>183</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>81</v>
@@ -3010,7 +3007,7 @@
         <v>382</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>626</v>
+        <v>614</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -3018,10 +3015,10 @@
         <v>63</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>95</v>
@@ -3051,21 +3048,21 @@
         <v>208</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>130</v>
@@ -3092,7 +3089,7 @@
         <v>246</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>628</v>
+        <v>616</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -3100,7 +3097,7 @@
         <v>287</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>115</v>
@@ -3133,18 +3130,18 @@
         <v>368</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>629</v>
+        <v>617</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>239</v>
@@ -3174,7 +3171,7 @@
         <v>202</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>630</v>
+        <v>618</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -3182,13 +3179,13 @@
         <v>139</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>92</v>
@@ -3215,7 +3212,7 @@
         <v>367</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>631</v>
+        <v>619</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -3223,7 +3220,7 @@
         <v>229</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>66</v>
@@ -3256,7 +3253,7 @@
         <v>383</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -3264,10 +3261,10 @@
         <v>104</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>326</v>
@@ -3297,15 +3294,15 @@
         <v>379</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>633</v>
+        <v>621</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="3" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>76</v>
@@ -3338,21 +3335,21 @@
         <v>209</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>634</v>
+        <v>622</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>379</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>140</v>
@@ -3379,7 +3376,7 @@
         <v>375</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>635</v>
+        <v>623</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -3387,7 +3384,7 @@
         <v>135</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>129</v>
@@ -3420,21 +3417,21 @@
         <v>204</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>636</v>
+        <v>624</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="3" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>45</v>
@@ -3461,7 +3458,7 @@
         <v>203</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>637</v>
+        <v>625</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -3469,10 +3466,10 @@
         <v>86</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>67</v>
@@ -3499,7 +3496,7 @@
         <v>197</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>638</v>
+        <v>626</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -3507,7 +3504,7 @@
         <v>350</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>79</v>
@@ -3537,7 +3534,7 @@
         <v>84</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -3545,7 +3542,7 @@
         <v>365</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>165</v>
@@ -3575,7 +3572,7 @@
         <v>199</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>640</v>
+        <v>628</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -3583,13 +3580,13 @@
         <v>171</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>5</v>
@@ -3613,15 +3610,15 @@
         <v>214</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>641</v>
+        <v>629</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="3" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>150</v>
@@ -3651,15 +3648,15 @@
         <v>373</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>642</v>
+        <v>630</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="3" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>207</v>
@@ -3689,7 +3686,7 @@
         <v>37</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>643</v>
+        <v>631</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -3697,10 +3694,10 @@
         <v>82</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>316</v>
@@ -3727,7 +3724,7 @@
         <v>177</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>644</v>
+        <v>632</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -3735,13 +3732,13 @@
         <v>130</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>61</v>
@@ -3762,7 +3759,7 @@
         <v>377</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>645</v>
+        <v>633</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -3770,10 +3767,10 @@
         <v>223</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>31</v>
@@ -3795,7 +3792,7 @@
         <v>364</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>646</v>
+        <v>634</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -3803,10 +3800,10 @@
         <v>41</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>47</v>
@@ -3824,18 +3821,18 @@
         <v>380</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>647</v>
+        <v>635</v>
       </c>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="3" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>44</v>
@@ -3854,7 +3851,7 @@
         <v>372</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>648</v>
+        <v>636</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -3862,10 +3859,10 @@
         <v>200</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>275</v>
@@ -3883,15 +3880,15 @@
         <v>371</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>649</v>
+        <v>637</v>
       </c>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="3" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>309</v>
@@ -3909,7 +3906,7 @@
         <v>370</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>650</v>
+        <v>638</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -4011,7 +4008,7 @@
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="3" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>29</v>
@@ -4045,7 +4042,7 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="3" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>80</v>
@@ -4076,7 +4073,7 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="3" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>123</v>
@@ -4132,7 +4129,7 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="3" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>95</v>
@@ -4160,7 +4157,7 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="3" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>93</v>
@@ -4174,7 +4171,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="3" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>109</v>
@@ -4188,7 +4185,7 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="3" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>30</v>
@@ -4277,7 +4274,7 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="3" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>70</v>
@@ -4288,7 +4285,7 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="3" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>106</v>
@@ -4321,7 +4318,7 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="3" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>77</v>
@@ -4332,7 +4329,7 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>6</v>
@@ -4387,7 +4384,7 @@
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="3" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>115</v>
@@ -4398,7 +4395,7 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="3" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>116</v>
@@ -4420,7 +4417,7 @@
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>133</v>
@@ -4431,7 +4428,7 @@
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="3" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>42</v>
@@ -4464,7 +4461,7 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="3" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>33</v>
@@ -4475,7 +4472,7 @@
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>100</v>
@@ -4497,7 +4494,7 @@
     </row>
     <row r="85" spans="1:12">
       <c r="A85" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>46</v>
@@ -4596,7 +4593,7 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="3" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>2</v>
@@ -4607,7 +4604,7 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>48</v>
@@ -4618,7 +4615,7 @@
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="3" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>53</v>
@@ -4629,7 +4626,7 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>21</v>
@@ -4662,7 +4659,7 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>112</v>
@@ -4673,7 +4670,7 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="3" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>129</v>
@@ -4695,7 +4692,7 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="3" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>35</v>
@@ -4728,7 +4725,7 @@
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="3" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>78</v>
@@ -4739,7 +4736,7 @@
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="3" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>79</v>
@@ -4761,7 +4758,7 @@
     </row>
     <row r="109" spans="1:12">
       <c r="A109" s="3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>43</v>
@@ -4783,7 +4780,7 @@
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>68</v>
@@ -4849,7 +4846,7 @@
     </row>
     <row r="117" spans="1:12">
       <c r="A117" s="3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>107</v>
@@ -4871,7 +4868,7 @@
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="3" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="E119" s="4" t="s">
         <v>0</v>
@@ -4937,7 +4934,7 @@
     </row>
     <row r="125" spans="1:12">
       <c r="A125" s="3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>57</v>
@@ -4959,7 +4956,7 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>125</v>
@@ -5003,7 +5000,7 @@
     </row>
     <row r="131" spans="1:12">
       <c r="A131" s="3" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>132</v>
@@ -5014,7 +5011,7 @@
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>119</v>
@@ -5025,7 +5022,7 @@
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>55</v>
@@ -5047,7 +5044,7 @@
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>72</v>
@@ -5124,7 +5121,7 @@
     </row>
     <row r="142" spans="1:12">
       <c r="A142" s="3" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>89</v>
@@ -5162,7 +5159,7 @@
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="3" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="L146" s="2" t="s">
         <v>284</v>
@@ -5170,7 +5167,7 @@
     </row>
     <row r="147" spans="1:12">
       <c r="A147" s="3" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="L147" s="4" t="s">
         <v>275</v>
@@ -5178,7 +5175,7 @@
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="3" t="s">
-        <v>499</v>
+        <v>639</v>
       </c>
       <c r="L148" s="2" t="s">
         <v>309</v>
@@ -5202,7 +5199,7 @@
     </row>
     <row r="151" spans="1:12">
       <c r="A151" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="L151" s="2" t="s">
         <v>277</v>
@@ -5226,7 +5223,7 @@
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="3" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="L154" s="2" t="s">
         <v>323</v>
@@ -5234,7 +5231,7 @@
     </row>
     <row r="155" spans="1:12">
       <c r="A155" s="3" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="L155" s="2" t="s">
         <v>311</v>
@@ -5250,7 +5247,7 @@
     </row>
     <row r="157" spans="1:12">
       <c r="A157" s="3" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="L157" s="2" t="s">
         <v>320</v>
@@ -5274,7 +5271,7 @@
     </row>
     <row r="160" spans="1:12">
       <c r="A160" s="3" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="L160" s="2" t="s">
         <v>347</v>
@@ -5310,12 +5307,12 @@
     </row>
     <row r="166" spans="1:12">
       <c r="A166" s="3" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="167" spans="1:12">
       <c r="A167" s="3" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="168" spans="1:12">
@@ -5325,7 +5322,7 @@
     </row>
     <row r="169" spans="1:12">
       <c r="A169" s="3" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="170" spans="1:12">
@@ -5335,12 +5332,12 @@
     </row>
     <row r="171" spans="1:12">
       <c r="A171" s="3" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="172" spans="1:12">
       <c r="A172" s="3" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="173" spans="1:12">
@@ -5350,7 +5347,7 @@
     </row>
     <row r="174" spans="1:12">
       <c r="A174" s="3" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="175" spans="1:12">
@@ -5365,12 +5362,12 @@
     </row>
     <row r="177" spans="1:1">
       <c r="A177" s="3" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" s="3" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="179" spans="1:1">
@@ -5380,7 +5377,7 @@
     </row>
     <row r="180" spans="1:1">
       <c r="A180" s="3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="181" spans="1:1">
@@ -5400,17 +5397,17 @@
     </row>
     <row r="184" spans="1:1">
       <c r="A184" s="3" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" s="3" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="187" spans="1:1">
@@ -5420,7 +5417,7 @@
     </row>
     <row r="188" spans="1:1">
       <c r="A188" s="3" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="189" spans="1:1">
@@ -5445,17 +5442,17 @@
     </row>
     <row r="193" spans="1:1">
       <c r="A193" s="3" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" s="3" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" s="3" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="196" spans="1:1">
@@ -5480,12 +5477,12 @@
     </row>
     <row r="200" spans="1:1">
       <c r="A200" s="3" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" s="3" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="202" spans="1:1">
@@ -5495,12 +5492,12 @@
     </row>
     <row r="203" spans="1:1">
       <c r="A203" s="3" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" s="3" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="205" spans="1:1">
@@ -5510,7 +5507,7 @@
     </row>
     <row r="206" spans="1:1">
       <c r="A206" s="3" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="207" spans="1:1">
@@ -5520,12 +5517,12 @@
     </row>
     <row r="208" spans="1:1">
       <c r="A208" s="3" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" s="3" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="210" spans="1:1">
@@ -5535,7 +5532,7 @@
     </row>
     <row r="211" spans="1:1">
       <c r="A211" s="3" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="212" spans="1:1">
@@ -5545,12 +5542,12 @@
     </row>
     <row r="213" spans="1:1">
       <c r="A213" s="3" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" s="3" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="215" spans="1:1">
@@ -5560,22 +5557,22 @@
     </row>
     <row r="216" spans="1:1">
       <c r="A216" s="3" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" s="3" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" s="3" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" s="3" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="220" spans="1:1">
@@ -5585,7 +5582,7 @@
     </row>
     <row r="221" spans="1:1">
       <c r="A221" s="3" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="222" spans="1:1">
@@ -5600,7 +5597,7 @@
     </row>
     <row r="224" spans="1:1">
       <c r="A224" s="3" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="225" spans="1:1">
@@ -5625,7 +5622,7 @@
     </row>
     <row r="229" spans="1:1">
       <c r="A229" s="3" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="230" spans="1:1">
@@ -5635,12 +5632,12 @@
     </row>
     <row r="231" spans="1:1">
       <c r="A231" s="3" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" s="3" t="s">
-        <v>533</v>
+        <v>640</v>
       </c>
     </row>
     <row r="233" spans="1:1">
@@ -5665,7 +5662,7 @@
     </row>
     <row r="237" spans="1:1">
       <c r="A237" s="3" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
     </row>
     <row r="238" spans="1:1">
@@ -5685,17 +5682,17 @@
     </row>
     <row r="241" spans="1:1">
       <c r="A241" s="3" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" s="3" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" s="3" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
     </row>
     <row r="244" spans="1:1">
@@ -5710,17 +5707,17 @@
     </row>
     <row r="246" spans="1:1">
       <c r="A246" s="3" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" s="3" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" s="3" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="249" spans="1:1">
@@ -5730,7 +5727,7 @@
     </row>
     <row r="250" spans="1:1">
       <c r="A250" s="3" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="251" spans="1:1">
@@ -5750,7 +5747,7 @@
     </row>
     <row r="254" spans="1:1">
       <c r="A254" s="3" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="255" spans="1:1">
@@ -5765,7 +5762,7 @@
     </row>
     <row r="257" spans="1:1">
       <c r="A257" s="3" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
     </row>
     <row r="258" spans="1:1">
@@ -5775,7 +5772,7 @@
     </row>
     <row r="259" spans="1:1">
       <c r="A259" s="3" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="260" spans="1:1">
@@ -5785,7 +5782,7 @@
     </row>
     <row r="261" spans="1:1">
       <c r="A261" s="3" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
     </row>
     <row r="262" spans="1:1">
@@ -5795,7 +5792,7 @@
     </row>
     <row r="263" spans="1:1">
       <c r="A263" s="3" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
     </row>
     <row r="264" spans="1:1">
@@ -5805,7 +5802,7 @@
     </row>
     <row r="265" spans="1:1">
       <c r="A265" s="3" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
     </row>
     <row r="266" spans="1:1">
@@ -5825,32 +5822,32 @@
     </row>
     <row r="269" spans="1:1">
       <c r="A269" s="3" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" s="3" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" s="3" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" s="3" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" s="3" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" s="3" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
     </row>
     <row r="275" spans="1:1">
@@ -5875,7 +5872,7 @@
     </row>
     <row r="279" spans="1:1">
       <c r="A279" s="3" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
     </row>
     <row r="280" spans="1:1">
@@ -5890,7 +5887,7 @@
     </row>
     <row r="282" spans="1:1">
       <c r="A282" s="3" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="283" spans="1:1">
@@ -5905,7 +5902,7 @@
     </row>
     <row r="285" spans="1:1">
       <c r="A285" s="3" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="286" spans="1:1">
@@ -5915,12 +5912,12 @@
     </row>
     <row r="287" spans="1:1">
       <c r="A287" s="3" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" s="3" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
     <row r="289" spans="1:1">
@@ -5940,7 +5937,7 @@
     </row>
     <row r="292" spans="1:1">
       <c r="A292" s="3" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
     </row>
     <row r="293" spans="1:1">
@@ -5965,37 +5962,37 @@
     </row>
     <row r="297" spans="1:1">
       <c r="A297" s="3" t="s">
-        <v>558</v>
+        <v>641</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" s="3" t="s">
-        <v>559</v>
+        <v>642</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" s="3" t="s">
-        <v>560</v>
+        <v>643</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" s="3" t="s">
-        <v>561</v>
+        <v>644</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" s="3" t="s">
-        <v>562</v>
+        <v>645</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" s="3" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" s="3" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
     </row>
     <row r="304" spans="1:1">
@@ -6015,12 +6012,12 @@
     </row>
     <row r="307" spans="1:1">
       <c r="A307" s="3" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" s="3" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
     </row>
     <row r="309" spans="1:1">
@@ -6050,7 +6047,7 @@
     </row>
     <row r="314" spans="1:1">
       <c r="A314" s="3" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
     </row>
     <row r="315" spans="1:1">
@@ -6065,7 +6062,7 @@
     </row>
     <row r="317" spans="1:1">
       <c r="A317" s="3" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="318" spans="1:1">
@@ -6080,12 +6077,12 @@
     </row>
     <row r="320" spans="1:1">
       <c r="A320" s="3" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" s="3" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
     </row>
     <row r="322" spans="1:1">
@@ -6105,17 +6102,17 @@
     </row>
     <row r="325" spans="1:1">
       <c r="A325" s="3" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" s="3" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" s="3" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
     </row>
     <row r="328" spans="1:1">
@@ -6135,7 +6132,7 @@
     </row>
     <row r="331" spans="1:1">
       <c r="A331" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="332" spans="1:1">
@@ -6145,17 +6142,17 @@
     </row>
     <row r="333" spans="1:1">
       <c r="A333" s="3" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" s="3" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="336" spans="1:1">
@@ -6175,7 +6172,7 @@
     </row>
     <row r="339" spans="1:1">
       <c r="A339" s="3" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
     </row>
     <row r="340" spans="1:1">
@@ -6220,12 +6217,12 @@
     </row>
     <row r="348" spans="1:1">
       <c r="A348" s="3" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" s="3" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
     </row>
     <row r="350" spans="1:1">
@@ -6245,32 +6242,32 @@
     </row>
     <row r="353" spans="1:1">
       <c r="A353" s="3" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" s="3" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" s="3" t="s">
-        <v>580</v>
+        <v>570</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" s="3" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" s="3" t="s">
-        <v>581</v>
+        <v>571</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" s="3" t="s">
-        <v>582</v>
+        <v>572</v>
       </c>
     </row>
     <row r="359" spans="1:1">
@@ -6285,27 +6282,27 @@
     </row>
     <row r="361" spans="1:1">
       <c r="A361" s="3" t="s">
-        <v>583</v>
+        <v>573</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" s="3" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" s="3" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" s="3" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" s="3" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="366" spans="1:1">
@@ -6315,12 +6312,12 @@
     </row>
     <row r="367" spans="1:1">
       <c r="A367" s="3" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" s="3" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
     </row>
     <row r="369" spans="1:1">
@@ -6330,12 +6327,12 @@
     </row>
     <row r="370" spans="1:1">
       <c r="A370" s="3" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" s="3" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
     </row>
     <row r="372" spans="1:1">
@@ -6360,17 +6357,17 @@
     </row>
     <row r="376" spans="1:1">
       <c r="A376" s="3" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" s="3" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" s="3" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
     </row>
     <row r="379" spans="1:1">
@@ -6385,7 +6382,7 @@
     </row>
     <row r="381" spans="1:1">
       <c r="A381" s="3" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
     </row>
     <row r="382" spans="1:1">
@@ -6405,22 +6402,22 @@
     </row>
     <row r="385" spans="1:1">
       <c r="A385" s="3" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" s="3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" s="3" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" s="3" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
     </row>
     <row r="389" spans="1:1">
@@ -6430,7 +6427,7 @@
     </row>
     <row r="390" spans="1:1">
       <c r="A390" s="3" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
     </row>
     <row r="391" spans="1:1">
@@ -6440,12 +6437,12 @@
     </row>
     <row r="392" spans="1:1">
       <c r="A392" s="3" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" s="3" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
     </row>
     <row r="394" spans="1:1">
@@ -6475,12 +6472,12 @@
     </row>
     <row r="399" spans="1:1">
       <c r="A399" s="3" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" s="3" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
     </row>
     <row r="401" spans="1:1">
@@ -6490,12 +6487,12 @@
     </row>
     <row r="402" spans="1:1">
       <c r="A402" s="3" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" s="3" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
     </row>
     <row r="404" spans="1:1">
@@ -6505,51 +6502,61 @@
     </row>
     <row r="405" spans="1:1">
       <c r="A405" s="3" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" s="3" t="s">
-        <v>606</v>
+        <v>89</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" s="3" t="s">
-        <v>607</v>
+        <v>88</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" s="3" t="s">
-        <v>384</v>
+        <v>87</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" s="3" t="s">
-        <v>320</v>
+        <v>596</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" s="3" t="s">
-        <v>288</v>
+        <v>384</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" s="3" t="s">
-        <v>608</v>
+        <v>320</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" s="3" t="s">
-        <v>348</v>
+        <v>288</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" s="3" t="s">
-        <v>263</v>
+        <v>597</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1">
+      <c r="A415" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1">
+      <c r="A416" s="3" t="s">
         <v>273</v>
       </c>
     </row>
@@ -6694,7 +6701,7 @@
     <hyperlink ref="A364" r:id="rId134" tooltip="Togekiss"/>
     <hyperlink ref="A387" r:id="rId135" tooltip="Victini"/>
     <hyperlink ref="A394" r:id="rId136" tooltip="Volcarona"/>
-    <hyperlink ref="A414" r:id="rId137" tooltip="Zygarde"/>
+    <hyperlink ref="A416" r:id="rId137" tooltip="Zygarde"/>
     <hyperlink ref="A14" r:id="rId138" tooltip="Arcanine"/>
     <hyperlink ref="A23" r:id="rId139" tooltip="Azelf"/>
     <hyperlink ref="A37" r:id="rId140" tooltip="Blissey"/>
@@ -6741,7 +6748,7 @@
     <hyperlink ref="A273" r:id="rId181" tooltip="Porygon2"/>
     <hyperlink ref="A292" r:id="rId182" tooltip="Reuniclus"/>
     <hyperlink ref="A296" r:id="rId183" tooltip="Roserade"/>
-    <hyperlink ref="A300" r:id="rId184" tooltip="Rotom"/>
+    <hyperlink ref="A300" r:id="rId184" tooltip="Rotom" display="Rotom-H (Heat Form)"/>
     <hyperlink ref="A303" r:id="rId185" tooltip="Sableye"/>
     <hyperlink ref="A304" r:id="rId186" tooltip="Salamence"/>
     <hyperlink ref="A320" r:id="rId187" tooltip="Shaymin"/>
@@ -6755,7 +6762,7 @@
     <hyperlink ref="A382" r:id="rId195" tooltip="Vaporeon"/>
     <hyperlink ref="A384" r:id="rId196" tooltip="Venusaur"/>
     <hyperlink ref="A402" r:id="rId197" tooltip="Whimsicott"/>
-    <hyperlink ref="A410" r:id="rId198" tooltip="Zapdos"/>
+    <hyperlink ref="A412" r:id="rId198" tooltip="Zapdos"/>
     <hyperlink ref="A86" r:id="rId199" tooltip="Dragalge"/>
     <hyperlink ref="A123" r:id="rId200" tooltip="Froslass"/>
     <hyperlink ref="A184" r:id="rId201" tooltip="Kingdra"/>
@@ -6766,8 +6773,8 @@
     <hyperlink ref="A323" r:id="rId206" tooltip="Shuckle"/>
     <hyperlink ref="A367" r:id="rId207" tooltip="Tornadus"/>
     <hyperlink ref="A383" r:id="rId208" tooltip="Venomoth"/>
-    <hyperlink ref="A408" r:id="rId209" tooltip="Yanmega"/>
-    <hyperlink ref="A412" r:id="rId210" tooltip="Zoroark"/>
+    <hyperlink ref="A410" r:id="rId209" tooltip="Yanmega"/>
+    <hyperlink ref="A414" r:id="rId210" tooltip="Zoroark"/>
     <hyperlink ref="A2" r:id="rId211" tooltip="Abomasnow"/>
     <hyperlink ref="A3" r:id="rId212" tooltip="Absol"/>
     <hyperlink ref="A4" r:id="rId213" tooltip="Accelgor"/>
@@ -6811,7 +6818,7 @@
     <hyperlink ref="A281" r:id="rId251" tooltip="Qwilfish"/>
     <hyperlink ref="A290" r:id="rId252" tooltip="Registeel"/>
     <hyperlink ref="A294" r:id="rId253" tooltip="Rhyperior"/>
-    <hyperlink ref="A298" r:id="rId254" tooltip="Rotom"/>
+    <hyperlink ref="A298" r:id="rId254" tooltip="Rotom" display="Rotom-C (Lawn Mower form)"/>
     <hyperlink ref="A312" r:id="rId255" tooltip="Scrafty"/>
     <hyperlink ref="A315" r:id="rId256" tooltip="Seismitoad"/>
     <hyperlink ref="A319" r:id="rId257" tooltip="Sharpedo"/>
@@ -6871,8 +6878,8 @@
     <hyperlink ref="A279" r:id="rId311" tooltip="Quagsire"/>
     <hyperlink ref="A289" r:id="rId312" tooltip="Regirock"/>
     <hyperlink ref="A293" r:id="rId313" tooltip="Rhydon"/>
-    <hyperlink ref="A297" r:id="rId314" tooltip="Rotom"/>
-    <hyperlink ref="A301" r:id="rId315" tooltip="Rotom"/>
+    <hyperlink ref="A297" r:id="rId314" tooltip="Rotom" display="Rotom (Normal form)"/>
+    <hyperlink ref="A301" r:id="rId315" tooltip="Rotom" display="Rotom-S (Fan form)"/>
     <hyperlink ref="A305" r:id="rId316" tooltip="Samurott"/>
     <hyperlink ref="A306" r:id="rId317" tooltip="Sandslash"/>
     <hyperlink ref="A307" r:id="rId318" tooltip="Sawk"/>
@@ -6887,8 +6894,8 @@
     <hyperlink ref="A390" r:id="rId327" tooltip="Vileplume"/>
     <hyperlink ref="A392" r:id="rId328" tooltip="Vivillon"/>
     <hyperlink ref="A401" r:id="rId329" tooltip="Weezing"/>
-    <hyperlink ref="A407" r:id="rId330" tooltip="Xatu"/>
-    <hyperlink ref="A409" r:id="rId331" tooltip="Zangoose"/>
+    <hyperlink ref="A409" r:id="rId330" tooltip="Xatu"/>
+    <hyperlink ref="A411" r:id="rId331" tooltip="Zangoose"/>
     <hyperlink ref="A26" r:id="rId332" tooltip="Barbaracle"/>
     <hyperlink ref="A47" r:id="rId333" tooltip="Carracosta"/>
     <hyperlink ref="A205" r:id="rId334" tooltip="Linoone"/>
@@ -6953,7 +6960,7 @@
     <hyperlink ref="A143" r:id="rId393" tooltip="Golem"/>
     <hyperlink ref="A146" r:id="rId394" tooltip="Gorebyss"/>
     <hyperlink ref="A147" r:id="rId395" tooltip="Gothitelle"/>
-    <hyperlink ref="A148" r:id="rId396" tooltip="Gourgeist"/>
+    <hyperlink ref="A148" r:id="rId396" tooltip="Gourgeist" display="Gourgeist (all forms)"/>
     <hyperlink ref="A150" r:id="rId397" tooltip="Grumpig"/>
     <hyperlink ref="A157" r:id="rId398" tooltip="Heatmor"/>
     <hyperlink ref="A169" r:id="rId399" tooltip="Huntail"/>
@@ -6981,7 +6988,7 @@
     <hyperlink ref="A226" r:id="rId421" tooltip="Marowak"/>
     <hyperlink ref="A227" r:id="rId422" tooltip="Masquerain"/>
     <hyperlink ref="A230" r:id="rId423" tooltip="Meganium"/>
-    <hyperlink ref="A232" r:id="rId424" tooltip="Meowstic"/>
+    <hyperlink ref="A232" r:id="rId424" tooltip="Meowstic" display="Meowstic (Both Male and Female)"/>
     <hyperlink ref="A235" r:id="rId425" tooltip="Metang"/>
     <hyperlink ref="A238" r:id="rId426" tooltip="Mightyena"/>
     <hyperlink ref="A241" r:id="rId427" tooltip="Minun"/>
@@ -7014,7 +7021,7 @@
     <hyperlink ref="A288" r:id="rId454" tooltip="Regigigas"/>
     <hyperlink ref="A291" r:id="rId455" tooltip="Relicanth"/>
     <hyperlink ref="A295" r:id="rId456" tooltip="Roselia"/>
-    <hyperlink ref="A299" r:id="rId457" tooltip="Rotom"/>
+    <hyperlink ref="A299" r:id="rId457" tooltip="Rotom" display="Rotom-F (Freezer form)"/>
     <hyperlink ref="A308" r:id="rId458" tooltip="Sawsbuck"/>
     <hyperlink ref="A314" r:id="rId459" tooltip="Seaking"/>
     <hyperlink ref="A317" r:id="rId460" tooltip="Servine"/>
@@ -7053,9 +7060,9 @@
     <hyperlink ref="A403" r:id="rId493" tooltip="Whiscash"/>
     <hyperlink ref="A404" r:id="rId494" tooltip="Wigglytuff"/>
     <hyperlink ref="A405" r:id="rId495" tooltip="Wobbuffet"/>
-    <hyperlink ref="A406" r:id="rId496" tooltip="Wormadam"/>
-    <hyperlink ref="A411" r:id="rId497" tooltip="Zebstrika"/>
-    <hyperlink ref="A413" r:id="rId498" tooltip="Zweilous"/>
+    <hyperlink ref="A408" r:id="rId496" tooltip="Wormadam" display="Wormadam (All Forms)"/>
+    <hyperlink ref="A413" r:id="rId497" tooltip="Zebstrika"/>
+    <hyperlink ref="A415" r:id="rId498" tooltip="Zweilous"/>
     <hyperlink ref="B6" r:id="rId499" tooltip="Mega Alakazam"/>
     <hyperlink ref="B7" r:id="rId500" tooltip="Mega Altaria"/>
     <hyperlink ref="B14" r:id="rId501" tooltip="Mega Charizard X"/>

</xml_diff>